<commit_message>
Updated documents for Gantt Chart
</commit_message>
<xml_diff>
--- a/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLab_repo\documents\Published\GanttChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="BVT" sheetId="4" r:id="rId1"/>
+    <sheet name="Checklist" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <r>
       <t>#</t>
@@ -171,12 +173,266 @@
   <si>
     <t>Does visual legends adjusted on resizing? </t>
   </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>BVT</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>A Gantt chart with specified categories should be created.</t>
+  </si>
+  <si>
+    <t>Display basic Gantt chart</t>
+  </si>
+  <si>
+    <t>1. Drag 'Region', 'Metro','ProjectName' and 'Tranche' in 'Category' field
+2. Drag 'MilestonePhaseStart' in 'Start' field
+3. Drag 'MilestonePhaseFinish' in 'End' field</t>
+  </si>
+  <si>
+    <t>Data labels for each bar should be displayed.</t>
+  </si>
+  <si>
+    <t>KPI Data</t>
+  </si>
+  <si>
+    <t>Display Gantt chart with Data label</t>
+  </si>
+  <si>
+    <t>Display Gantt chart with KPI Data</t>
+  </si>
+  <si>
+    <t>A KPI Section in Gantt Chart should be displayed.</t>
+  </si>
+  <si>
+    <t>Tooltip Data</t>
+  </si>
+  <si>
+    <t>Display Gantt chart with Tooltip on Bars</t>
+  </si>
+  <si>
+    <t>S no</t>
+  </si>
+  <si>
+    <t>Expected output</t>
+  </si>
+  <si>
+    <t>Basic chart</t>
+  </si>
+  <si>
+    <t>1. Drag 'Region', 'Metro','ProjectName' and 'Tranche' in 'Category' field
+2. Drag 'MilestonePhaseStart' in 'Start' field
+3. Drag 'MilestonePhaseFinish' in 'End' field
+4. Drag 'Dest' column in 'Data Label' field</t>
+  </si>
+  <si>
+    <t>1. Drag 'Region', 'Metro','ProjectName' and 'Tranche' in 'Category' field
+2. Drag 'MilestonePhaseStart' in 'Start' field
+3. Drag 'MilestonePhaseFinish' in 'End' field
+4. Drag 'SafetyStatus' column in 'KPI' field</t>
+  </si>
+  <si>
+    <t>1. Drag 'Region', 'Metro','ProjectName' and 'Tranche' in 'Category' field
+2. Drag 'MilestonePhaseStart' in 'Start' field
+3. Drag 'MilestonePhaseFinish' in 'End' field
+4. Drag 'ProjectName' column in 'Tooltip' field</t>
+  </si>
+  <si>
+    <t>A tooltip on hover of each bar with Project name should be displayed.</t>
+  </si>
+  <si>
+    <t>Legend settings</t>
+  </si>
+  <si>
+    <t>Column headers settings</t>
+  </si>
+  <si>
+    <t>Horizontal scroll position settings</t>
+  </si>
+  <si>
+    <t>KPI column type settings</t>
+  </si>
+  <si>
+    <t>Gantt date type settings</t>
+  </si>
+  <si>
+    <t>Grid lines settings</t>
+  </si>
+  <si>
+    <t>Display ratio settings</t>
+  </si>
+  <si>
+    <t>Category labels settings</t>
+  </si>
+  <si>
+    <t>Display legends in chart</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Legends' option
+3. Switch the toggle on-off</t>
+  </si>
+  <si>
+    <t>Display or hide legends in chart</t>
+  </si>
+  <si>
+    <t>Update Font color, Background color, Outline, Font family and Text size</t>
+  </si>
+  <si>
+    <t>1. 'Font color' will be set to 'red'
+2. 'Background color' will be set to 'black'
+3. 'Outline' will be added for column headers as a 'Frame'
+4. 'Font family' will be set to 'Arial Black'
+5. 'Text size' will be set to '30'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Column headers' option
+3. Update 'Font color' to 'red'
+4. Update 'Background color' to 'black'
+5. Update 'Outline' to 'Frame'
+6. Update 'Font family' to 'Arial Black'
+7. Update 'Text size' to '30'</t>
+  </si>
+  <si>
+    <t>Display Data labels in chart</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Data labels' option
+3. Switch the toggle on-off</t>
+  </si>
+  <si>
+    <t>Display or hide Data labels in chart</t>
+  </si>
+  <si>
+    <t>Update Position, Color, Text size, Font family</t>
+  </si>
+  <si>
+    <t>Update Type and Show today indicator</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Data labels' option
+3. Switch the toggle on
+4. Update 'Position' to 'Right'
+5. Update 'Color' to 'red'
+6. Update 'Text size' to '30'
+7. Update 'Font family' to 'Arial Black'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Gantt date type' option
+3. Update 'Type' to 'Month'
+4. Update 'Show today indicator' to 'On'</t>
+  </si>
+  <si>
+    <t>1. 'Type' will be set to 'Month'
+2. Today indicator will be added to chart</t>
+  </si>
+  <si>
+    <t>Update Horizontal scroll position</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Horizontal scroll position' option
+3. Update 'Position' to 'Today'</t>
+  </si>
+  <si>
+    <t>1. 'Position' will be set to 'Today'. Scroll bar will be moved to today line.</t>
+  </si>
+  <si>
+    <t>Update KPI Column type</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'KPI column type' option
+3. Update 'SafetyStatus' to 'Indicator'
+4. Update 'SafetyStatus' to 'Type'</t>
+  </si>
+  <si>
+    <t>Display Grid lines in chart</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Grid lines' option
+3. Switch the toggle on-off</t>
+  </si>
+  <si>
+    <t>Display or hide Grid lines in chart</t>
+  </si>
+  <si>
+    <t>Update Color, Interval</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Grid lines' option
+3. Switch the toggle on
+4. Update 'Color' to 'red'
+5. Update 'Interval' to '3'</t>
+  </si>
+  <si>
+    <t>1. 'SafetyStatus' will be set to 'Indicator'
+2. 'SafetyStatus' will be set to 'Type'</t>
+  </si>
+  <si>
+    <t>Update Ratio</t>
+  </si>
+  <si>
+    <t>1. Display Grid lines in chart
+2. 'Color' will be set to 'red'
+3. 'Interval' will be set to '3'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Display ratio' option
+3. Update 'Ratio' to '50%'</t>
+  </si>
+  <si>
+    <t>1. 'Ratio' will be set to '50%'</t>
+  </si>
+  <si>
+    <t>Update Font color, Text size, Font family, Is Expanded, Hierarchy layout</t>
+  </si>
+  <si>
+    <t>1. 'Font color' will be set to 'red'
+2. 'Text size' will be set to '30'
+3. 'Font family' will be set to 'Arial Black'
+4. Category labels section should be collapsed
+5. Category labels will be displayed in a hierarchical manner</t>
+  </si>
+  <si>
+    <t>1. Data labels will be displayed in chart
+2. 'Position' will be set to 'Right'
+3. 'Color' will be set to 'red'
+4. 'Text size' will be set to 30
+5. 'Font family' will be set to 'Arial Black'</t>
+  </si>
+  <si>
+    <t>Data labels settings</t>
+  </si>
+  <si>
+    <t>Data Labels Data</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Category labels' option
+3. Update 'Font color' to 'red'
+4. Update 'Text size' to '30'
+5. Update 'Font family' to 'Arial Black'
+6. Update 'IsExpanded' to 'On'
+7. Update 'Hierarchy layout' to 'On'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +451,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -306,6 +570,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -638,10 +908,295 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="47" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>13</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0726AE0-5413-4F42-B05F-1BEAC53441DD}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -828,29 +1383,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
@@ -864,41 +1419,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="12">
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="14"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">

</xml_diff>